<commit_message>
added in fixed effects
</commit_message>
<xml_diff>
--- a/COVIDPPP/simple_regression2.xlsx
+++ b/COVIDPPP/simple_regression2.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Justin\Gov50\pppdata\COVIDPPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E74A90-6E81-4787-9715-410E3600065F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F76E7B7-5B15-4C0C-804A-A5CA651D2C14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5C0248D8-EA7F-4B58-AE6F-972E3FB6C12F}"/>
   </bookViews>
   <sheets>
     <sheet name="zip" sheetId="1" r:id="rId1"/>
-    <sheet name="county" sheetId="2" r:id="rId2"/>
+    <sheet name="zip2" sheetId="3" r:id="rId2"/>
+    <sheet name="county" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="121">
   <si>
     <t>Model 1</t>
   </si>
@@ -341,6 +342,63 @@
   </si>
   <si>
     <t>Regressor</t>
+  </si>
+  <si>
+    <t>0.086***</t>
+  </si>
+  <si>
+    <t>0.065***</t>
+  </si>
+  <si>
+    <t>0.048***</t>
+  </si>
+  <si>
+    <t>0.022***</t>
+  </si>
+  <si>
+    <t>0.021</t>
+  </si>
+  <si>
+    <t>(0.006)</t>
+  </si>
+  <si>
+    <t>(0.020)</t>
+  </si>
+  <si>
+    <t>0.000*</t>
+  </si>
+  <si>
+    <t>0.011</t>
+  </si>
+  <si>
+    <t>-0.019</t>
+  </si>
+  <si>
+    <t>(0.040)</t>
+  </si>
+  <si>
+    <t>R2 (full model)</t>
+  </si>
+  <si>
+    <t>0.050</t>
+  </si>
+  <si>
+    <t>0.311</t>
+  </si>
+  <si>
+    <t>0.556</t>
+  </si>
+  <si>
+    <t>0.811</t>
+  </si>
+  <si>
+    <t>Adj. R2 (full model)</t>
+  </si>
+  <si>
+    <t>0.049</t>
+  </si>
+  <si>
+    <t>0.310</t>
   </si>
 </sst>
 </file>
@@ -1193,11 +1251,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A13939-F957-46CE-ADB4-928E2E1F7DF1}">
-  <dimension ref="A1:F25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A33397-649D-49F9-B366-14D09A9F4F06}">
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1227,6 +1285,447 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A13939-F957-46CE-ADB4-928E2E1F7DF1}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">

</xml_diff>